<commit_message>
preparar para subir a render
</commit_message>
<xml_diff>
--- a/datos_bot.xlsx
+++ b/datos_bot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R3nE8\Documents\Programacion\PrinterBoy\chatbot_printerboy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52188923-A768-45CD-BDA4-79518C855BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15C0DB0-FA21-4235-93DF-1B1757D67C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{BB83B82B-A6BF-4B56-8C1D-28A46D4FF631}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB83B82B-A6BF-4B56-8C1D-28A46D4FF631}"/>
   </bookViews>
   <sheets>
     <sheet name="Productos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
   <si>
     <t>Precio</t>
   </si>
@@ -105,27 +105,15 @@
     <t>Impresion a blanco y negro</t>
   </si>
   <si>
-    <t>Lona</t>
-  </si>
-  <si>
     <t>Engomado</t>
   </si>
   <si>
-    <t>¿Que precio tiene una lona de X tamaño?</t>
-  </si>
-  <si>
-    <t>¿cuanto cuesta una lona de tamaño x tamaño?</t>
-  </si>
-  <si>
     <t>Sucursal</t>
   </si>
   <si>
     <t>Ubicacion</t>
   </si>
   <si>
-    <t>formula: (tamaño) * (tamaño) * 210</t>
-  </si>
-  <si>
     <t>Explicacion</t>
   </si>
   <si>
@@ -304,6 +292,27 @@
   </si>
   <si>
     <t>sin informacion</t>
+  </si>
+  <si>
+    <t>En cuanto sale una lona de (tamaño) x (tamaño)?</t>
+  </si>
+  <si>
+    <t>¿cuanto cuesta una lona de (tamaño) x (tamaño)?</t>
+  </si>
+  <si>
+    <t>¿Que precio tiene una lona de (tamaño)?</t>
+  </si>
+  <si>
+    <t>si solo te especifican un tamaño significa que vas a multiplicar ese tamaño x 1 metro por defecto: formula: (tamaño) * 1 * 210</t>
+  </si>
+  <si>
+    <t>si te piden una lona de 2 medidas (ancho y largo) la formula es: (tamaño) * (tamaño) * 210</t>
+  </si>
+  <si>
+    <t>Lonas (lona)</t>
+  </si>
+  <si>
+    <t>se vende por metro lineal</t>
   </si>
 </sst>
 </file>
@@ -681,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A532DCC-344E-494B-A3FE-DC3947968A3A}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -707,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3">
         <v>7</v>
@@ -718,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -729,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C4" s="3">
         <v>8</v>
@@ -740,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C5" s="3">
         <v>3</v>
@@ -751,7 +760,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3">
         <v>7</v>
@@ -762,7 +771,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C7" s="3">
         <v>2</v>
@@ -770,10 +779,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3">
         <v>15</v>
@@ -781,10 +790,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" s="3">
         <v>15</v>
@@ -792,10 +801,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3">
         <v>10</v>
@@ -803,10 +812,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3">
         <v>18</v>
@@ -817,7 +826,7 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3">
         <v>10</v>
@@ -828,7 +837,7 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C13" s="3">
         <v>10</v>
@@ -836,10 +845,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="C14" s="3">
         <v>210</v>
@@ -847,10 +856,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3">
         <v>30</v>
@@ -858,10 +867,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3">
         <v>45</v>
@@ -869,10 +878,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3">
         <v>50</v>
@@ -880,10 +889,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3">
         <v>65</v>
@@ -891,10 +900,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19" s="3">
         <v>45</v>
@@ -902,10 +911,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" s="3">
         <v>250</v>
@@ -913,10 +922,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C21" s="3">
         <v>100</v>
@@ -924,10 +933,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C22" s="3">
         <v>450</v>
@@ -935,10 +944,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C23" s="3">
         <v>600</v>
@@ -946,10 +955,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C24" s="3">
         <v>650</v>
@@ -957,10 +966,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C25" s="3">
         <v>800</v>
@@ -968,10 +977,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3">
         <v>450</v>
@@ -979,10 +988,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C27" s="3">
         <v>200</v>
@@ -990,10 +999,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3">
         <v>420</v>
@@ -1001,10 +1010,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C29" s="3">
         <v>630</v>
@@ -1012,10 +1021,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C30" s="3">
         <v>60</v>
@@ -1023,10 +1032,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C31" s="3">
         <v>110</v>
@@ -1034,10 +1043,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C32" s="3">
         <v>210</v>
@@ -1045,10 +1054,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C33" s="3">
         <v>12</v>
@@ -1056,10 +1065,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C34" s="3">
         <v>2</v>
@@ -1067,10 +1076,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C35" s="3">
         <v>14</v>
@@ -1078,10 +1087,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C36" s="3">
         <v>6</v>
@@ -1089,10 +1098,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C37" s="3">
         <v>12</v>
@@ -1100,10 +1109,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C38" s="3">
         <v>2</v>
@@ -1111,10 +1120,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C39" s="3">
         <v>25</v>
@@ -1122,10 +1131,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C40" s="3">
         <v>23</v>
@@ -1133,10 +1142,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C41" s="3">
         <v>15</v>
@@ -1144,10 +1153,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C42" s="3">
         <v>28</v>
@@ -1155,10 +1164,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C43" s="3">
         <v>20</v>
@@ -1166,10 +1175,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C44" s="3">
         <v>20</v>
@@ -1177,10 +1186,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C45" s="3">
         <v>8</v>
@@ -1188,10 +1197,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C46" s="3">
         <v>12</v>
@@ -1199,10 +1208,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C47" s="3">
         <v>12</v>
@@ -1210,10 +1219,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C48" s="3">
         <v>20</v>
@@ -1221,10 +1230,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C49" s="3">
         <v>4</v>
@@ -1232,10 +1241,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C50" s="3">
         <v>9</v>
@@ -1243,10 +1252,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C51" s="3">
         <v>6</v>
@@ -1254,10 +1263,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C52" s="3">
         <v>14</v>
@@ -1288,13 +1297,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>6</v>
@@ -1305,10 +1314,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -1325,7 +1334,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -1339,13 +1348,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
         <v>84</v>
       </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D4">
         <v>6535170204</v>
@@ -1356,16 +1365,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
         <v>87</v>
-      </c>
-      <c r="C5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" t="s">
-        <v>91</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -1430,40 +1439,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3511174F-3C8D-484F-AF10-527540AA2A27}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.33203125" customWidth="1"/>
-    <col min="2" max="2" width="51.77734375" customWidth="1"/>
+    <col min="2" max="2" width="117.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1472,6 +1481,14 @@
       </c>
       <c r="B4" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>